<commit_message>
db setup pipeline config
</commit_message>
<xml_diff>
--- a/notes/Class inventory.xlsx
+++ b/notes/Class inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\john\projects\appinsight\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA836AE-D67A-481C-BCC8-57B9BCE7EFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE1ECE2-DAD4-4EB5-BB8D-F2B2808B7D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40125" yWindow="4410" windowWidth="33945" windowHeight="15555" xr2:uid="{73B4164B-88E2-47A3-B1A7-5683065D2BD2}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="173">
   <si>
     <t>Layer</t>
   </si>
@@ -517,28 +517,34 @@
     <t>pending</t>
   </si>
   <si>
-    <t>DatasetDBSetupTask</t>
-  </si>
-  <si>
-    <t>BackupDBSetupTask</t>
-  </si>
-  <si>
-    <t>ProfileDBSetupTask</t>
-  </si>
-  <si>
-    <t>Sets up the Dataset DB</t>
-  </si>
-  <si>
-    <t>Sets up the backup DB</t>
-  </si>
-  <si>
-    <t>Sets up the profile DB</t>
-  </si>
-  <si>
     <t>closed</t>
   </si>
   <si>
     <t>Not needed</t>
+  </si>
+  <si>
+    <t>DatasetDBSetupConfig</t>
+  </si>
+  <si>
+    <t>ProfileDBSetupConfig</t>
+  </si>
+  <si>
+    <t>BackupDBSetupConfig</t>
+  </si>
+  <si>
+    <t>Sets up the dataset table</t>
+  </si>
+  <si>
+    <t>Sets up the profile table</t>
+  </si>
+  <si>
+    <t>Sets up the backup table</t>
+  </si>
+  <si>
+    <t>DatasetFileSetupConfig</t>
+  </si>
+  <si>
+    <t>Dataset file setup config</t>
   </si>
 </sst>
 </file>
@@ -890,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFDCAF8C-AED9-42D5-9A1C-3140A47EB069}">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,7 +1167,7 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="F9" t="s">
         <v>159</v>
@@ -1184,28 +1190,28 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>165</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>168</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
       </c>
       <c r="I10" t="s">
-        <v>74</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1213,31 +1219,28 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
         <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>166</v>
       </c>
       <c r="G11" t="s">
-        <v>76</v>
+        <v>169</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
       </c>
       <c r="I11" t="s">
         <v>122</v>
-      </c>
-      <c r="K11" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1245,31 +1248,28 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
       <c r="F12" t="s">
-        <v>78</v>
+        <v>167</v>
       </c>
       <c r="G12" t="s">
-        <v>79</v>
+        <v>170</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
       </c>
       <c r="I12" t="s">
         <v>122</v>
-      </c>
-      <c r="K12" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1280,25 +1280,25 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>118</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>123</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>124</v>
+        <v>71</v>
       </c>
       <c r="G13" t="s">
-        <v>125</v>
+        <v>73</v>
       </c>
       <c r="H13" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I13" t="s">
-        <v>121</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1309,25 +1309,28 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>118</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>61</v>
       </c>
       <c r="F14" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="G14" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
       </c>
       <c r="I14" t="s">
-        <v>121</v>
+        <v>122</v>
+      </c>
+      <c r="K14" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1338,19 +1341,19 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="F15" t="s">
-        <v>163</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="H15" t="s">
         <v>15</v>
@@ -1358,68 +1361,71 @@
       <c r="I15" t="s">
         <v>122</v>
       </c>
+      <c r="K15" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="F16" t="s">
-        <v>164</v>
+        <v>124</v>
       </c>
       <c r="G16" t="s">
-        <v>167</v>
+        <v>125</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="F17" t="s">
-        <v>165</v>
+        <v>126</v>
       </c>
       <c r="G17" t="s">
-        <v>168</v>
+        <v>127</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
       </c>
       <c r="I17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -1448,7 +1454,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -1477,7 +1483,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -1506,7 +1512,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
@@ -1535,7 +1541,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -1564,7 +1570,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -1593,7 +1599,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
@@ -1622,7 +1628,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
@@ -1634,45 +1640,45 @@
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="F25" t="s">
-        <v>119</v>
+        <v>157</v>
       </c>
       <c r="G25" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="H25" t="s">
         <v>15</v>
       </c>
       <c r="I25" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="D26" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="G26" t="s">
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="H26" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I26" t="s">
         <v>121</v>
@@ -1680,36 +1686,36 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>117</v>
+        <v>50</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F27" t="s">
-        <v>115</v>
+        <v>53</v>
       </c>
       <c r="G27" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="H27" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I27" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
@@ -1718,16 +1724,16 @@
         <v>44</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G28" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H28" t="s">
         <v>15</v>
@@ -1738,7 +1744,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -1753,10 +1759,10 @@
         <v>10</v>
       </c>
       <c r="F29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H29" t="s">
         <v>15</v>
@@ -1767,7 +1773,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
@@ -1776,27 +1782,27 @@
         <v>44</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="G30" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="H30" t="s">
         <v>15</v>
       </c>
       <c r="I30" t="s">
-        <v>121</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
@@ -1811,10 +1817,10 @@
         <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H31" t="s">
         <v>15</v>
@@ -1825,7 +1831,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
@@ -1837,24 +1843,24 @@
         <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F32" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G32" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H32" t="s">
         <v>15</v>
       </c>
       <c r="I32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
@@ -1869,82 +1875,82 @@
         <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H33" t="s">
         <v>15</v>
       </c>
       <c r="I33" t="s">
-        <v>169</v>
-      </c>
-      <c r="K33" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>118</v>
+        <v>44</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>157</v>
+        <v>64</v>
       </c>
       <c r="G34" t="s">
-        <v>156</v>
+        <v>46</v>
       </c>
       <c r="H34" t="s">
         <v>15</v>
       </c>
       <c r="I34" t="s">
-        <v>122</v>
+        <v>163</v>
+      </c>
+      <c r="K34" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E35" t="s">
         <v>82</v>
       </c>
       <c r="F35" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="G35" t="s">
-        <v>19</v>
+        <v>161</v>
       </c>
       <c r="H35" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I35" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
         <v>49</v>
@@ -1956,13 +1962,13 @@
         <v>16</v>
       </c>
       <c r="E36" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="F36" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G36" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H36" t="s">
         <v>20</v>
@@ -1973,68 +1979,68 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>49</v>
       </c>
       <c r="C37" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="E37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>67</v>
+        <v>154</v>
       </c>
       <c r="G37" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="H37" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I37" t="s">
-        <v>121</v>
-      </c>
-      <c r="K37" t="s">
-        <v>70</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
         <v>49</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="D38" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E38" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F38" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="G38" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="H38" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I38" t="s">
-        <v>74</v>
+        <v>121</v>
+      </c>
+      <c r="K38" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
         <v>49</v>
@@ -2049,10 +2055,10 @@
         <v>17</v>
       </c>
       <c r="F39" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G39" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H39" t="s">
         <v>20</v>
@@ -2063,7 +2069,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
         <v>49</v>
@@ -2075,16 +2081,16 @@
         <v>82</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F40" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G40" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H40" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I40" t="s">
         <v>74</v>
@@ -2092,7 +2098,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
         <v>49</v>
@@ -2104,13 +2110,13 @@
         <v>82</v>
       </c>
       <c r="E41" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="F41" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H41" t="s">
         <v>15</v>
@@ -2121,7 +2127,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
         <v>49</v>
@@ -2130,16 +2136,16 @@
         <v>81</v>
       </c>
       <c r="D42" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="E42" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="F42" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="G42" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="H42" t="s">
         <v>15</v>
@@ -2150,7 +2156,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
         <v>49</v>
@@ -2159,16 +2165,16 @@
         <v>81</v>
       </c>
       <c r="D43" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E43" t="s">
-        <v>84</v>
+        <v>9</v>
       </c>
       <c r="F43" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="G43" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="H43" t="s">
         <v>15</v>
@@ -2179,7 +2185,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
         <v>49</v>
@@ -2191,13 +2197,13 @@
         <v>10</v>
       </c>
       <c r="E44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G44" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H44" t="s">
         <v>15</v>
@@ -2208,7 +2214,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
         <v>49</v>
@@ -2217,19 +2223,19 @@
         <v>81</v>
       </c>
       <c r="D45" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="F45" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="G45" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="H45" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I45" t="s">
         <v>74</v>
@@ -2237,7 +2243,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
         <v>49</v>
@@ -2246,19 +2252,19 @@
         <v>81</v>
       </c>
       <c r="D46" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="E46" t="s">
-        <v>102</v>
+        <v>17</v>
       </c>
       <c r="F46" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G46" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H46" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I46" t="s">
         <v>74</v>
@@ -2266,7 +2272,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
         <v>49</v>
@@ -2281,10 +2287,10 @@
         <v>102</v>
       </c>
       <c r="F47" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G47" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H47" t="s">
         <v>15</v>
@@ -2295,7 +2301,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
         <v>49</v>
@@ -2307,13 +2313,13 @@
         <v>98</v>
       </c>
       <c r="E48" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F48" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G48" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H48" t="s">
         <v>15</v>
@@ -2324,36 +2330,36 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
         <v>49</v>
       </c>
       <c r="C49" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="D49" t="s">
-        <v>140</v>
+        <v>98</v>
       </c>
       <c r="E49" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="F49" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="G49" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
       <c r="H49" t="s">
         <v>15</v>
       </c>
       <c r="I49" t="s">
-        <v>121</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
         <v>49</v>
@@ -2362,27 +2368,27 @@
         <v>16</v>
       </c>
       <c r="D50" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="E50" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F50" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="G50" t="s">
-        <v>56</v>
+        <v>142</v>
       </c>
       <c r="H50" t="s">
         <v>15</v>
       </c>
       <c r="I50" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
         <v>49</v>
@@ -2391,27 +2397,27 @@
         <v>16</v>
       </c>
       <c r="D51" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="E51" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F51" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H51" t="s">
         <v>15</v>
       </c>
       <c r="I51" t="s">
-        <v>121</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
         <v>49</v>
@@ -2420,60 +2426,89 @@
         <v>16</v>
       </c>
       <c r="D52" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="G52" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H52" t="s">
         <v>15</v>
       </c>
       <c r="I52" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>49</v>
+      </c>
+      <c r="C53" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" t="s">
+        <v>50</v>
+      </c>
+      <c r="E53" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" t="s">
         <v>51</v>
       </c>
-      <c r="B53" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" t="s">
-        <v>44</v>
-      </c>
-      <c r="D53" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" t="s">
-        <v>82</v>
-      </c>
-      <c r="F53" t="s">
-        <v>160</v>
-      </c>
       <c r="G53" t="s">
-        <v>161</v>
+        <v>55</v>
       </c>
       <c r="H53" t="s">
         <v>15</v>
       </c>
       <c r="I53" t="s">
-        <v>121</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
+        <v>50</v>
+      </c>
+      <c r="E54" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" t="s">
+        <v>171</v>
+      </c>
+      <c r="G54" t="s">
+        <v>172</v>
+      </c>
+      <c r="H54" t="s">
+        <v>15</v>
+      </c>
+      <c r="I54" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K52">
-    <sortCondition ref="B2:B52"/>
-    <sortCondition ref="C2:C52"/>
-    <sortCondition ref="D2:D52"/>
-    <sortCondition ref="E2:E52"/>
-    <sortCondition ref="F2:F52"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K53">
+    <sortCondition ref="B2:B53"/>
+    <sortCondition ref="C2:C53"/>
+    <sortCondition ref="D2:D53"/>
+    <sortCondition ref="E2:E53"/>
+    <sortCondition ref="F2:F53"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>